<commit_message>
Enabled ability to have posting label in a separate worksheet from the data
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
+++ b/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B20BB9-878D-4549-A3FF-8291FEBE7833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D483C99-4E6C-4EA3-A44D-4FD595E5DC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -923,7 +923,7 @@
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2577,6 +2577,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F6243DC9F1A5042A9E247A4534B7346" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d7c915ce63f17b192f15f9b5c7111dd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="16245bed-a411-4918-92cd-ff4510683069" xmlns:ns3="ddeece39-a33c-49ad-a8fd-0ae9fa2c3195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="06dc0855dc4fc49148f60a39d2bf92c3" ns2:_="" ns3:_="">
     <xsd:import namespace="16245bed-a411-4918-92cd-ff4510683069"/>
@@ -2793,22 +2808,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22B48C8D-ED50-492C-9680-7011CC9B9CB9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2825,21 +2842,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Progressed with big rocks posting functionality for variant=explained. Still need to finish it
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
+++ b/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/simple_burnout_INPUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317C9B4B-1911-44E6-80CA-0DEEF637DA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC239E80-89FF-4E4E-BDCC-52A7CA8E2565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7327" yWindow="3885" windowWidth="12578" windowHeight="11715" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
   <sheets>
     <sheet name="simple burnout" sheetId="5" r:id="rId1"/>
@@ -203,9 +203,6 @@
     <t>broken; explained</t>
   </si>
   <si>
-    <t>simple; burnout</t>
-  </si>
-  <si>
     <t>FusionOpus</t>
   </si>
   <si>
@@ -264,6 +261,9 @@
   </si>
   <si>
     <t>delivery-planning.journeys.a6i.io/v1a</t>
+  </si>
+  <si>
+    <t>burnout</t>
   </si>
 </sst>
 </file>
@@ -923,7 +923,7 @@
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -943,7 +943,7 @@
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2"/>
       <c r="E1" s="3" t="s">
@@ -958,10 +958,10 @@
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>75</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>0</v>
@@ -971,10 +971,10 @@
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>58</v>
       </c>
       <c r="J2" s="24" t="s">
         <v>53</v>
@@ -986,7 +986,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>31</v>
@@ -1061,7 +1061,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>34</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>0</v>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B9" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
@@ -1137,10 +1137,10 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B10" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13">
@@ -1154,10 +1154,10 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B11" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B12" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1182,20 +1182,20 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B13" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B14" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1299,7 +1299,7 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
@@ -1318,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="38"/>
       <c r="E2" s="35" t="s">
@@ -1335,10 +1335,10 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>58</v>
       </c>
       <c r="L2" s="24" t="s">
         <v>53</v>
@@ -1697,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2"/>
       <c r="E1" s="3" t="s">
@@ -1709,7 +1709,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>0</v>
@@ -1798,7 +1798,7 @@
         <v>50</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>33</v>
@@ -2079,7 +2079,7 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2"/>
       <c r="E1" s="3" t="s">
@@ -2091,7 +2091,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="24" t="s">
         <v>0</v>
@@ -2577,18 +2577,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2809,18 +2809,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>